<commit_message>
working on veg data
</commit_message>
<xml_diff>
--- a/Veg_species_list_AI_07222022.xlsx
+++ b/Veg_species_list_AI_07222022.xlsx
@@ -8,15 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alissaiverson/.ssh/HLC_soil_and_veg/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8FC9E8D-C82C-D147-9F70-65DA3FDC384B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67FE29D-F3FE-EF4E-A8E3-041D4C754198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Export" sheetId="1" r:id="rId1"/>
     <sheet name="Formatted" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1850,7 +1862,7 @@
   <dimension ref="A1:F58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>